<commit_message>
Add column ST to Excel
</commit_message>
<xml_diff>
--- a/Listado CT.xlsx
+++ b/Listado CT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Descarga-de-Cuentas-Tributarias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705EA686-9A3B-4190-9D2E-51518084595F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D787A2D-F7AB-47F2-816A-84CB6D093535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Listado!$A$1:$Q$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Listado!$A$1:$R$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="21">
   <si>
     <t>Nro</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -2215,7 +2221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2230,13 +2236,14 @@
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2265,31 +2272,34 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f t="shared" ref="A2:A33" si="0">RIGHT(D2,1)</f>
         <v>0</v>
@@ -2309,7 +2319,7 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
@@ -2319,40 +2329,43 @@
         <f>H2&amp;B2&amp;"\"</f>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J2" s="2" t="str">
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="str">
         <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CT - ",SUBSTITUTE(D2,"-","")," - ",B2," - ",YEAR(F2)&amp;"-"&amp;TEXT(MONTH(F2),"00")&amp;"-"&amp;TEXT(DAY(F2),"00"),".xlsx")</f>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K2" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L2" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D2&amp;" - "&amp;TEXT(F2,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L2" s="4" t="e">
+      <c r="M2" s="4" t="e">
         <f>VLOOKUP(C2,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M2" s="4" t="e">
-        <f t="shared" ref="M2:M33" si="1">IF(EXACT(L2,E2),"ü","x")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N2" s="4">
-        <f t="shared" ref="N2:N33" si="2">ROW(A2)</f>
+      <c r="N2" s="4" t="e">
+        <f t="shared" ref="N2:N33" si="1">IF(EXACT(M2,E2),"ü","x")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O2" s="4">
+        <f t="shared" ref="O2:O33" si="2">ROW(A2)</f>
         <v>2</v>
       </c>
-      <c r="O2" s="4">
-        <f t="shared" ref="O2:O33" si="3">IF(C2=C1,1,0)</f>
-        <v>0</v>
-      </c>
       <c r="P2" s="4">
-        <f t="shared" ref="P2:P33" si="4">IF(C2=C3,1,0)</f>
-        <v>1</v>
+        <f t="shared" ref="P2:P33" si="3">IF(C2=C1,1,0)</f>
+        <v>0</v>
       </c>
       <c r="Q2" s="4">
-        <f t="shared" ref="Q2:Q33" si="5">SUM(O2:P2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q2:Q33" si="4">IF(C2=C3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="4">
+        <f t="shared" ref="R2:R33" si="5">SUM(P2:Q2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2372,7 +2385,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
@@ -2382,40 +2395,43 @@
         <f t="shared" ref="I3:I66" si="7">H3&amp;B3&amp;"\"</f>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J66" ca="1" si="8">CONCATENATE(TEXT(A3,"0")," - ","CT - ",SUBSTITUTE(D3,"-","")," - ",B3," - ",YEAR(F3)&amp;"-"&amp;TEXT(MONTH(F3),"00")&amp;"-"&amp;TEXT(DAY(F3),"00"),".xlsx")</f>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K3" s="5" t="str">
+      <c r="J3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f t="shared" ref="K3:K66" ca="1" si="8">CONCATENATE(TEXT(A3,"0")," - ","CT - ",SUBSTITUTE(D3,"-","")," - ",B3," - ",YEAR(F3)&amp;"-"&amp;TEXT(MONTH(F3),"00")&amp;"-"&amp;TEXT(DAY(F3),"00"),".xlsx")</f>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L3" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D3&amp;" - "&amp;TEXT(F3,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L3" s="4" t="e">
+      <c r="M3" s="4" t="e">
         <f>VLOOKUP(C3,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M3" s="4" t="e">
+      <c r="N3" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2435,7 +2451,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
@@ -2445,40 +2461,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J4" s="2" t="str">
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K4" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L4" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D4&amp;" - "&amp;TEXT(F4,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L4" s="4" t="e">
+      <c r="M4" s="4" t="e">
         <f>VLOOKUP(C4,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M4" s="4" t="e">
+      <c r="N4" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2497,7 +2516,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
@@ -2507,40 +2526,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J5" s="2" t="str">
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K5" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L5" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D5&amp;" - "&amp;TEXT(F5,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L5" s="4" t="e">
+      <c r="M5" s="4" t="e">
         <f>VLOOKUP(C5,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M5" s="4" t="e">
+      <c r="N5" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2560,7 +2582,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
@@ -2570,40 +2592,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J6" s="2" t="str">
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K6" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L6" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D6&amp;" - "&amp;TEXT(F6,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L6" s="4" t="e">
+      <c r="M6" s="4" t="e">
         <f>VLOOKUP(C6,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M6" s="4" t="e">
+      <c r="N6" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P6" s="4">
+      <c r="Q6" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2623,7 +2648,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
@@ -2633,40 +2658,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="J7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K7" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L7" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D7&amp;" - "&amp;TEXT(F7,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L7" s="4" t="e">
+      <c r="M7" s="4" t="e">
         <f>VLOOKUP(C7,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M7" s="4" t="e">
+      <c r="N7" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P7" s="4">
+      <c r="Q7" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="R7" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2686,7 +2714,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
@@ -2696,40 +2724,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J8" s="2" t="str">
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K8" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L8" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D8&amp;" - "&amp;TEXT(F8,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L8" s="4" t="e">
+      <c r="M8" s="4" t="e">
         <f>VLOOKUP(C8,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M8" s="4" t="e">
+      <c r="N8" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P8" s="4">
+      <c r="Q8" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="R8" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2749,7 +2780,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
@@ -2759,40 +2790,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J9" s="2" t="str">
+      <c r="J9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K9" s="5" t="str">
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L9" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D9&amp;" - "&amp;TEXT(F9,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L9" s="4" t="e">
+      <c r="M9" s="4" t="e">
         <f>VLOOKUP(C9,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M9" s="4" t="e">
+      <c r="N9" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P9" s="4">
+      <c r="Q9" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="R9" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2811,7 +2845,7 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
@@ -2821,40 +2855,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="J10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K10" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L10" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D10&amp;" - "&amp;TEXT(F10,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L10" s="4" t="e">
+      <c r="M10" s="4" t="e">
         <f>VLOOKUP(C10,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M10" s="4" t="e">
+      <c r="N10" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P10" s="4">
+      <c r="Q10" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="R10" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2873,7 +2910,7 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
@@ -2883,40 +2920,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="J11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K11" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L11" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D11&amp;" - "&amp;TEXT(F11,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L11" s="4" t="e">
+      <c r="M11" s="4" t="e">
         <f>VLOOKUP(C11,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M11" s="4" t="e">
+      <c r="N11" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="O11" s="4">
+      <c r="P11" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P11" s="4">
+      <c r="Q11" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="R11" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2935,7 +2975,7 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
@@ -2945,40 +2985,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J12" s="2" t="str">
+      <c r="J12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K12" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L12" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D12&amp;" - "&amp;TEXT(F12,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L12" s="4" t="e">
+      <c r="M12" s="4" t="e">
         <f>VLOOKUP(C12,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M12" s="4" t="e">
+      <c r="N12" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P12" s="4">
+      <c r="Q12" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="R12" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2997,7 +3040,7 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
@@ -3007,40 +3050,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J13" s="2" t="str">
+      <c r="J13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K13" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L13" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D13&amp;" - "&amp;TEXT(F13,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L13" s="4" t="e">
+      <c r="M13" s="4" t="e">
         <f>VLOOKUP(C13,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M13" s="4" t="e">
+      <c r="N13" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P13" s="4">
+      <c r="Q13" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3059,7 +3105,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
@@ -3069,40 +3115,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J14" s="2" t="str">
+      <c r="J14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K14" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L14" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D14&amp;" - "&amp;TEXT(F14,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L14" s="4" t="e">
+      <c r="M14" s="4" t="e">
         <f>VLOOKUP(C14,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M14" s="4" t="e">
+      <c r="N14" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P14" s="4">
+      <c r="Q14" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="R14" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3121,7 +3170,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
@@ -3131,40 +3180,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J15" s="2" t="str">
+      <c r="J15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K15" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L15" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D15&amp;" - "&amp;TEXT(F15,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L15" s="4" t="e">
+      <c r="M15" s="4" t="e">
         <f>VLOOKUP(C15,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M15" s="4" t="e">
+      <c r="N15" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="O15" s="4">
+      <c r="P15" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P15" s="4">
+      <c r="Q15" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="R15" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3183,7 +3235,7 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
@@ -3193,40 +3245,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J16" s="2" t="str">
+      <c r="J16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K16" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L16" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D16&amp;" - "&amp;TEXT(F16,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L16" s="4" t="e">
+      <c r="M16" s="4" t="e">
         <f>VLOOKUP(C16,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M16" s="4" t="e">
+      <c r="N16" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P16" s="4">
+      <c r="Q16" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="R16" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3245,7 +3300,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
@@ -3255,40 +3310,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J17" s="2" t="str">
+      <c r="J17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K17" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L17" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D17&amp;" - "&amp;TEXT(F17,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L17" s="4" t="e">
+      <c r="M17" s="4" t="e">
         <f>VLOOKUP(C17,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M17" s="4" t="e">
+      <c r="N17" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N17" s="4">
+      <c r="O17" s="4">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P17" s="4">
+      <c r="Q17" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R17" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3307,7 +3365,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
@@ -3317,40 +3375,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J18" s="2" t="str">
+      <c r="J18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K18" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L18" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D18&amp;" - "&amp;TEXT(F18,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L18" s="4" t="e">
+      <c r="M18" s="4" t="e">
         <f>VLOOKUP(C18,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M18" s="4" t="e">
+      <c r="N18" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N18" s="4">
+      <c r="O18" s="4">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="O18" s="4">
+      <c r="P18" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P18" s="4">
+      <c r="Q18" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="R18" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3369,7 +3430,7 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
@@ -3379,40 +3440,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J19" s="2" t="str">
+      <c r="J19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K19" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L19" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D19&amp;" - "&amp;TEXT(F19,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L19" s="4" t="e">
+      <c r="M19" s="4" t="e">
         <f>VLOOKUP(C19,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M19" s="4" t="e">
+      <c r="N19" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N19" s="4">
+      <c r="O19" s="4">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="O19" s="4">
+      <c r="P19" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P19" s="4">
+      <c r="Q19" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R19" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3431,7 +3495,7 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
@@ -3441,40 +3505,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J20" s="2" t="str">
+      <c r="J20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K20" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L20" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D20&amp;" - "&amp;TEXT(F20,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L20" s="4" t="e">
+      <c r="M20" s="4" t="e">
         <f>VLOOKUP(C20,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="4" t="e">
+      <c r="N20" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N20" s="4">
+      <c r="O20" s="4">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="O20" s="4">
+      <c r="P20" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P20" s="4">
+      <c r="Q20" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="R20" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3493,7 +3560,7 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
@@ -3503,40 +3570,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J21" s="2" t="str">
+      <c r="J21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K21" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L21" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D21&amp;" - "&amp;TEXT(F21,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L21" s="4" t="e">
+      <c r="M21" s="4" t="e">
         <f>VLOOKUP(C21,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M21" s="4" t="e">
+      <c r="N21" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N21" s="4">
+      <c r="O21" s="4">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="O21" s="4">
+      <c r="P21" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P21" s="4">
+      <c r="Q21" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="R21" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3555,7 +3625,7 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
@@ -3565,40 +3635,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J22" s="2" t="str">
+      <c r="J22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K22" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L22" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D22&amp;" - "&amp;TEXT(F22,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L22" s="4" t="e">
+      <c r="M22" s="4" t="e">
         <f>VLOOKUP(C22,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M22" s="4" t="e">
+      <c r="N22" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N22" s="4">
+      <c r="O22" s="4">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="O22" s="4">
+      <c r="P22" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P22" s="4">
+      <c r="Q22" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="R22" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3617,7 +3690,7 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
@@ -3627,40 +3700,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J23" s="2" t="str">
+      <c r="J23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K23" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L23" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D23&amp;" - "&amp;TEXT(F23,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L23" s="4" t="e">
+      <c r="M23" s="4" t="e">
         <f>VLOOKUP(C23,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M23" s="4" t="e">
+      <c r="N23" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N23" s="4">
+      <c r="O23" s="4">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="O23" s="4">
+      <c r="P23" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P23" s="4">
+      <c r="Q23" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="R23" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3679,7 +3755,7 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
@@ -3689,40 +3765,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J24" s="2" t="str">
+      <c r="J24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K24" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L24" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D24&amp;" - "&amp;TEXT(F24,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L24" s="4" t="e">
+      <c r="M24" s="4" t="e">
         <f>VLOOKUP(C24,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M24" s="4" t="e">
+      <c r="N24" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N24" s="4">
+      <c r="O24" s="4">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="O24" s="4">
+      <c r="P24" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P24" s="4">
+      <c r="Q24" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="R24" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3741,7 +3820,7 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
@@ -3751,40 +3830,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J25" s="2" t="str">
+      <c r="J25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K25" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L25" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D25&amp;" - "&amp;TEXT(F25,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L25" s="4" t="e">
+      <c r="M25" s="4" t="e">
         <f>VLOOKUP(C25,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M25" s="4" t="e">
+      <c r="N25" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N25" s="4">
+      <c r="O25" s="4">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="O25" s="4">
+      <c r="P25" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P25" s="4">
+      <c r="Q25" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="R25" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3803,7 +3885,7 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
@@ -3813,40 +3895,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J26" s="2" t="str">
+      <c r="J26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K26" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L26" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D26&amp;" - "&amp;TEXT(F26,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L26" s="4" t="e">
+      <c r="M26" s="4" t="e">
         <f>VLOOKUP(C26,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M26" s="4" t="e">
+      <c r="N26" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N26" s="4">
+      <c r="O26" s="4">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="O26" s="4">
+      <c r="P26" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P26" s="4">
+      <c r="Q26" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="R26" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3865,7 +3950,7 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
@@ -3875,40 +3960,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J27" s="2" t="str">
+      <c r="J27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K27" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L27" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D27&amp;" - "&amp;TEXT(F27,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L27" s="4" t="e">
+      <c r="M27" s="4" t="e">
         <f>VLOOKUP(C27,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M27" s="4" t="e">
+      <c r="N27" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N27" s="4">
+      <c r="O27" s="4">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="O27" s="4">
+      <c r="P27" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P27" s="4">
+      <c r="Q27" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="R27" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3927,7 +4015,7 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
@@ -3937,40 +4025,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J28" s="2" t="str">
+      <c r="J28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K28" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L28" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D28&amp;" - "&amp;TEXT(F28,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L28" s="4" t="e">
+      <c r="M28" s="4" t="e">
         <f>VLOOKUP(C28,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M28" s="4" t="e">
+      <c r="N28" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N28" s="4">
+      <c r="O28" s="4">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="O28" s="4">
+      <c r="P28" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P28" s="4">
+      <c r="Q28" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="R28" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3989,7 +4080,7 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
@@ -3999,40 +4090,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J29" s="2" t="str">
+      <c r="J29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K29" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L29" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D29&amp;" - "&amp;TEXT(F29,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L29" s="4" t="e">
+      <c r="M29" s="4" t="e">
         <f>VLOOKUP(C29,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M29" s="4" t="e">
+      <c r="N29" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N29" s="4">
+      <c r="O29" s="4">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="O29" s="4">
+      <c r="P29" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P29" s="4">
+      <c r="Q29" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="R29" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4051,7 +4145,7 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3" t="s">
@@ -4061,40 +4155,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J30" s="2" t="str">
+      <c r="J30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K30" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L30" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D30&amp;" - "&amp;TEXT(F30,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L30" s="4" t="e">
+      <c r="M30" s="4" t="e">
         <f>VLOOKUP(C30,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M30" s="4" t="e">
+      <c r="N30" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N30" s="4">
+      <c r="O30" s="4">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="O30" s="4">
+      <c r="P30" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P30" s="4">
+      <c r="Q30" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="R30" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4113,7 +4210,7 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
@@ -4123,40 +4220,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J31" s="2" t="str">
+      <c r="J31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K31" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L31" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D31&amp;" - "&amp;TEXT(F31,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L31" s="4" t="e">
+      <c r="M31" s="4" t="e">
         <f>VLOOKUP(C31,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M31" s="4" t="e">
+      <c r="N31" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N31" s="4">
+      <c r="O31" s="4">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="O31" s="4">
+      <c r="P31" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P31" s="4">
+      <c r="Q31" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="R31" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4175,7 +4275,7 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
@@ -4185,40 +4285,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J32" s="2" t="str">
+      <c r="J32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K32" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L32" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D32&amp;" - "&amp;TEXT(F32,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L32" s="4" t="e">
+      <c r="M32" s="4" t="e">
         <f>VLOOKUP(C32,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M32" s="4" t="e">
+      <c r="N32" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N32" s="4">
+      <c r="O32" s="4">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="O32" s="4">
+      <c r="P32" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P32" s="4">
+      <c r="Q32" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="R32" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4237,7 +4340,7 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
@@ -4247,40 +4350,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J33" s="2" t="str">
+      <c r="J33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K33" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L33" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D33&amp;" - "&amp;TEXT(F33,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L33" s="4" t="e">
+      <c r="M33" s="4" t="e">
         <f>VLOOKUP(C33,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M33" s="4" t="e">
+      <c r="N33" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N33" s="4">
+      <c r="O33" s="4">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="O33" s="4">
+      <c r="P33" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P33" s="4">
+      <c r="Q33" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="R33" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f t="shared" ref="A34:A69" si="9">RIGHT(D34,1)</f>
         <v>0</v>
@@ -4299,7 +4405,7 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
@@ -4309,40 +4415,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J34" s="2" t="str">
+      <c r="J34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K34" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L34" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D34&amp;" - "&amp;TEXT(F34,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L34" s="4" t="e">
+      <c r="M34" s="4" t="e">
         <f>VLOOKUP(C34,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M34" s="4" t="e">
-        <f t="shared" ref="M34:M65" si="10">IF(EXACT(L34,E34),"ü","x")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N34" s="4">
-        <f t="shared" ref="N34:N69" si="11">ROW(A34)</f>
+      <c r="N34" s="4" t="e">
+        <f t="shared" ref="N34:N65" si="10">IF(EXACT(M34,E34),"ü","x")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O34" s="4">
+        <f t="shared" ref="O34:O69" si="11">ROW(A34)</f>
         <v>34</v>
       </c>
-      <c r="O34" s="4">
-        <f t="shared" ref="O34:O67" si="12">IF(C34=C33,1,0)</f>
-        <v>1</v>
-      </c>
       <c r="P34" s="4">
-        <f t="shared" ref="P34:P67" si="13">IF(C34=C35,1,0)</f>
+        <f t="shared" ref="P34:P67" si="12">IF(C34=C33,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q34" s="4">
-        <f t="shared" ref="Q34:Q65" si="14">SUM(O34:P34)</f>
+        <f t="shared" ref="Q34:Q67" si="13">IF(C34=C35,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R34" s="4">
+        <f t="shared" ref="R34:R65" si="14">SUM(P34:Q34)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4361,7 +4470,7 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
@@ -4371,40 +4480,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J35" s="2" t="str">
+      <c r="J35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K35" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L35" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D35&amp;" - "&amp;TEXT(F35,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L35" s="4" t="e">
+      <c r="M35" s="4" t="e">
         <f>VLOOKUP(C35,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M35" s="4" t="e">
+      <c r="N35" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N35" s="4">
+      <c r="O35" s="4">
         <f t="shared" si="11"/>
         <v>35</v>
       </c>
-      <c r="O35" s="4">
+      <c r="P35" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P35" s="4">
+      <c r="Q35" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="R35" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4423,7 +4535,7 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3" t="s">
@@ -4433,40 +4545,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J36" s="2" t="str">
+      <c r="J36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K36" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L36" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D36&amp;" - "&amp;TEXT(F36,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L36" s="4" t="e">
+      <c r="M36" s="4" t="e">
         <f>VLOOKUP(C36,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M36" s="4" t="e">
+      <c r="N36" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N36" s="4">
+      <c r="O36" s="4">
         <f t="shared" si="11"/>
         <v>36</v>
       </c>
-      <c r="O36" s="4">
+      <c r="P36" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P36" s="4">
+      <c r="Q36" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q36" s="4">
+      <c r="R36" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4485,7 +4600,7 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3" t="s">
@@ -4495,40 +4610,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J37" s="2" t="str">
+      <c r="J37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K37" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L37" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D37&amp;" - "&amp;TEXT(F37,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L37" s="4" t="e">
+      <c r="M37" s="4" t="e">
         <f>VLOOKUP(C37,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M37" s="4" t="e">
+      <c r="N37" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N37" s="4">
+      <c r="O37" s="4">
         <f t="shared" si="11"/>
         <v>37</v>
       </c>
-      <c r="O37" s="4">
+      <c r="P37" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P37" s="4">
+      <c r="Q37" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q37" s="4">
+      <c r="R37" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4547,7 +4665,7 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3" t="s">
@@ -4557,40 +4675,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J38" s="2" t="str">
+      <c r="J38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K38" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L38" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D38&amp;" - "&amp;TEXT(F38,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L38" s="4" t="e">
+      <c r="M38" s="4" t="e">
         <f>VLOOKUP(C38,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M38" s="4" t="e">
+      <c r="N38" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N38" s="4">
+      <c r="O38" s="4">
         <f t="shared" si="11"/>
         <v>38</v>
       </c>
-      <c r="O38" s="4">
+      <c r="P38" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P38" s="4">
+      <c r="Q38" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q38" s="4">
+      <c r="R38" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4609,7 +4730,7 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3" t="s">
@@ -4619,40 +4740,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J39" s="2" t="str">
+      <c r="J39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K39" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L39" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D39&amp;" - "&amp;TEXT(F39,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L39" s="4" t="e">
+      <c r="M39" s="4" t="e">
         <f>VLOOKUP(C39,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M39" s="4" t="e">
+      <c r="N39" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N39" s="4">
+      <c r="O39" s="4">
         <f t="shared" si="11"/>
         <v>39</v>
       </c>
-      <c r="O39" s="4">
+      <c r="P39" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P39" s="4">
+      <c r="Q39" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="R39" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4671,7 +4795,7 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3" t="s">
@@ -4681,40 +4805,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J40" s="2" t="str">
+      <c r="J40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K40" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L40" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D40&amp;" - "&amp;TEXT(F40,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L40" s="4" t="e">
+      <c r="M40" s="4" t="e">
         <f>VLOOKUP(C40,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M40" s="4" t="e">
+      <c r="N40" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N40" s="4">
+      <c r="O40" s="4">
         <f t="shared" si="11"/>
         <v>40</v>
       </c>
-      <c r="O40" s="4">
+      <c r="P40" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P40" s="4">
+      <c r="Q40" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q40" s="4">
+      <c r="R40" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4733,7 +4860,7 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
@@ -4743,40 +4870,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J41" s="2" t="str">
+      <c r="J41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K41" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L41" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D41&amp;" - "&amp;TEXT(F41,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L41" s="4" t="e">
+      <c r="M41" s="4" t="e">
         <f>VLOOKUP(C41,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M41" s="4" t="e">
+      <c r="N41" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N41" s="4">
+      <c r="O41" s="4">
         <f t="shared" si="11"/>
         <v>41</v>
       </c>
-      <c r="O41" s="4">
+      <c r="P41" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P41" s="4">
+      <c r="Q41" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q41" s="4">
+      <c r="R41" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4795,7 +4925,7 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3" t="s">
@@ -4805,40 +4935,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J42" s="2" t="str">
+      <c r="J42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K42" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L42" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D42&amp;" - "&amp;TEXT(F42,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L42" s="4" t="e">
+      <c r="M42" s="4" t="e">
         <f>VLOOKUP(C42,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M42" s="4" t="e">
+      <c r="N42" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N42" s="4">
+      <c r="O42" s="4">
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="O42" s="4">
+      <c r="P42" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P42" s="4">
+      <c r="Q42" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q42" s="4">
+      <c r="R42" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4857,7 +4990,7 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3" t="s">
@@ -4867,40 +5000,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J43" s="2" t="str">
+      <c r="J43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K43" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L43" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D43&amp;" - "&amp;TEXT(F43,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L43" s="4" t="e">
+      <c r="M43" s="4" t="e">
         <f>VLOOKUP(C43,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M43" s="4" t="e">
+      <c r="N43" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N43" s="4">
+      <c r="O43" s="4">
         <f t="shared" si="11"/>
         <v>43</v>
       </c>
-      <c r="O43" s="4">
+      <c r="P43" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P43" s="4">
+      <c r="Q43" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q43" s="4">
+      <c r="R43" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4919,7 +5055,7 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3" t="s">
@@ -4929,40 +5065,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J44" s="2" t="str">
+      <c r="J44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K44" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L44" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D44&amp;" - "&amp;TEXT(F44,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L44" s="4" t="e">
+      <c r="M44" s="4" t="e">
         <f>VLOOKUP(C44,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M44" s="4" t="e">
+      <c r="N44" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N44" s="4">
+      <c r="O44" s="4">
         <f t="shared" si="11"/>
         <v>44</v>
       </c>
-      <c r="O44" s="4">
+      <c r="P44" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P44" s="4">
+      <c r="Q44" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q44" s="4">
+      <c r="R44" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4981,7 +5120,7 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
@@ -4991,40 +5130,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J45" s="2" t="str">
+      <c r="J45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K45" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L45" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D45&amp;" - "&amp;TEXT(F45,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L45" s="4" t="e">
+      <c r="M45" s="4" t="e">
         <f>VLOOKUP(C45,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M45" s="4" t="e">
+      <c r="N45" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N45" s="4">
+      <c r="O45" s="4">
         <f t="shared" si="11"/>
         <v>45</v>
       </c>
-      <c r="O45" s="4">
+      <c r="P45" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P45" s="4">
+      <c r="Q45" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q45" s="4">
+      <c r="R45" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5043,7 +5185,7 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
@@ -5053,40 +5195,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J46" s="2" t="str">
+      <c r="J46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K46" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L46" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D46&amp;" - "&amp;TEXT(F46,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L46" s="4" t="e">
+      <c r="M46" s="4" t="e">
         <f>VLOOKUP(C46,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M46" s="4" t="e">
+      <c r="N46" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N46" s="4">
+      <c r="O46" s="4">
         <f t="shared" si="11"/>
         <v>46</v>
       </c>
-      <c r="O46" s="4">
+      <c r="P46" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P46" s="4">
+      <c r="Q46" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q46" s="4">
+      <c r="R46" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5105,7 +5250,7 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3" t="s">
@@ -5115,40 +5260,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J47" s="2" t="str">
+      <c r="J47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K47" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L47" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D47&amp;" - "&amp;TEXT(F47,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L47" s="4" t="e">
+      <c r="M47" s="4" t="e">
         <f>VLOOKUP(C47,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M47" s="4" t="e">
+      <c r="N47" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N47" s="4">
+      <c r="O47" s="4">
         <f t="shared" si="11"/>
         <v>47</v>
       </c>
-      <c r="O47" s="4">
+      <c r="P47" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P47" s="4">
+      <c r="Q47" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q47" s="4">
+      <c r="R47" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5167,7 +5315,7 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3" t="s">
@@ -5177,40 +5325,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J48" s="2" t="str">
+      <c r="J48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K48" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L48" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D48&amp;" - "&amp;TEXT(F48,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L48" s="4" t="e">
+      <c r="M48" s="4" t="e">
         <f>VLOOKUP(C48,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M48" s="4" t="e">
+      <c r="N48" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N48" s="4">
+      <c r="O48" s="4">
         <f t="shared" si="11"/>
         <v>48</v>
       </c>
-      <c r="O48" s="4">
+      <c r="P48" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P48" s="4">
+      <c r="Q48" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q48" s="4">
+      <c r="R48" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5229,7 +5380,7 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3" t="s">
@@ -5239,40 +5390,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J49" s="2" t="str">
+      <c r="J49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K49" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L49" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D49&amp;" - "&amp;TEXT(F49,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L49" s="4" t="e">
+      <c r="M49" s="4" t="e">
         <f>VLOOKUP(C49,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M49" s="4" t="e">
+      <c r="N49" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N49" s="4">
+      <c r="O49" s="4">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="O49" s="4">
+      <c r="P49" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P49" s="4">
+      <c r="Q49" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q49" s="4">
+      <c r="R49" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5291,7 +5445,7 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3" t="s">
@@ -5301,40 +5455,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J50" s="2" t="str">
+      <c r="J50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K50" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L50" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D50&amp;" - "&amp;TEXT(F50,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L50" s="4" t="e">
+      <c r="M50" s="4" t="e">
         <f>VLOOKUP(C50,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M50" s="4" t="e">
+      <c r="N50" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N50" s="4">
+      <c r="O50" s="4">
         <f t="shared" si="11"/>
         <v>50</v>
       </c>
-      <c r="O50" s="4">
+      <c r="P50" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P50" s="4">
+      <c r="Q50" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q50" s="4">
+      <c r="R50" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5353,7 +5510,7 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3" t="s">
@@ -5363,40 +5520,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J51" s="2" t="str">
+      <c r="J51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K51" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L51" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D51&amp;" - "&amp;TEXT(F51,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L51" s="4" t="e">
+      <c r="M51" s="4" t="e">
         <f>VLOOKUP(C51,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M51" s="4" t="e">
+      <c r="N51" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N51" s="4">
+      <c r="O51" s="4">
         <f t="shared" si="11"/>
         <v>51</v>
       </c>
-      <c r="O51" s="4">
+      <c r="P51" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P51" s="4">
+      <c r="Q51" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q51" s="4">
+      <c r="R51" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5415,7 +5575,7 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3" t="s">
@@ -5425,40 +5585,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J52" s="2" t="str">
+      <c r="J52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K52" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L52" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D52&amp;" - "&amp;TEXT(F52,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L52" s="4" t="e">
+      <c r="M52" s="4" t="e">
         <f>VLOOKUP(C52,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M52" s="4" t="e">
+      <c r="N52" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N52" s="4">
+      <c r="O52" s="4">
         <f t="shared" si="11"/>
         <v>52</v>
       </c>
-      <c r="O52" s="4">
+      <c r="P52" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P52" s="4">
+      <c r="Q52" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q52" s="4">
+      <c r="R52" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5477,7 +5640,7 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3" t="s">
@@ -5487,40 +5650,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J53" s="2" t="str">
+      <c r="J53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K53" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L53" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D53&amp;" - "&amp;TEXT(F53,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L53" s="4" t="e">
+      <c r="M53" s="4" t="e">
         <f>VLOOKUP(C53,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M53" s="4" t="e">
+      <c r="N53" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N53" s="4">
+      <c r="O53" s="4">
         <f t="shared" si="11"/>
         <v>53</v>
       </c>
-      <c r="O53" s="4">
+      <c r="P53" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P53" s="4">
+      <c r="Q53" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q53" s="4">
+      <c r="R53" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5539,7 +5705,7 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3" t="s">
@@ -5549,40 +5715,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J54" s="2" t="str">
+      <c r="J54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K54" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L54" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D54&amp;" - "&amp;TEXT(F54,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L54" s="4" t="e">
+      <c r="M54" s="4" t="e">
         <f>VLOOKUP(C54,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M54" s="4" t="e">
+      <c r="N54" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N54" s="4">
+      <c r="O54" s="4">
         <f t="shared" si="11"/>
         <v>54</v>
       </c>
-      <c r="O54" s="4">
+      <c r="P54" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P54" s="4">
+      <c r="Q54" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q54" s="4">
+      <c r="R54" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5601,7 +5770,7 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3" t="s">
@@ -5611,40 +5780,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J55" s="2" t="str">
+      <c r="J55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K55" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L55" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D55&amp;" - "&amp;TEXT(F55,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L55" s="4" t="e">
+      <c r="M55" s="4" t="e">
         <f>VLOOKUP(C55,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M55" s="4" t="e">
+      <c r="N55" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N55" s="4">
+      <c r="O55" s="4">
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="O55" s="4">
+      <c r="P55" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P55" s="4">
+      <c r="Q55" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q55" s="4">
+      <c r="R55" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5663,7 +5835,7 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3" t="s">
@@ -5673,40 +5845,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J56" s="2" t="str">
+      <c r="J56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K56" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L56" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D56&amp;" - "&amp;TEXT(F56,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L56" s="4" t="e">
+      <c r="M56" s="4" t="e">
         <f>VLOOKUP(C56,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M56" s="4" t="e">
+      <c r="N56" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N56" s="4">
+      <c r="O56" s="4">
         <f t="shared" si="11"/>
         <v>56</v>
       </c>
-      <c r="O56" s="4">
+      <c r="P56" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P56" s="4">
+      <c r="Q56" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q56" s="4">
+      <c r="R56" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5725,7 +5900,7 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3" t="s">
@@ -5735,40 +5910,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J57" s="2" t="str">
+      <c r="J57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K57" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L57" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D57&amp;" - "&amp;TEXT(F57,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L57" s="4" t="e">
+      <c r="M57" s="4" t="e">
         <f>VLOOKUP(C57,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M57" s="4" t="e">
+      <c r="N57" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N57" s="4">
+      <c r="O57" s="4">
         <f t="shared" si="11"/>
         <v>57</v>
       </c>
-      <c r="O57" s="4">
+      <c r="P57" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P57" s="4">
+      <c r="Q57" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q57" s="4">
+      <c r="R57" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5787,7 +5965,7 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3" t="s">
@@ -5797,40 +5975,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J58" s="2" t="str">
+      <c r="J58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K58" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L58" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D58&amp;" - "&amp;TEXT(F58,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L58" s="4" t="e">
+      <c r="M58" s="4" t="e">
         <f>VLOOKUP(C58,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M58" s="4" t="e">
+      <c r="N58" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N58" s="4">
+      <c r="O58" s="4">
         <f t="shared" si="11"/>
         <v>58</v>
       </c>
-      <c r="O58" s="4">
+      <c r="P58" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P58" s="4">
+      <c r="Q58" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q58" s="4">
+      <c r="R58" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5849,7 +6030,7 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3" t="s">
@@ -5859,40 +6040,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J59" s="2" t="str">
+      <c r="J59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K59" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L59" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D59&amp;" - "&amp;TEXT(F59,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L59" s="4" t="e">
+      <c r="M59" s="4" t="e">
         <f>VLOOKUP(C59,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M59" s="4" t="e">
+      <c r="N59" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N59" s="4">
+      <c r="O59" s="4">
         <f t="shared" si="11"/>
         <v>59</v>
       </c>
-      <c r="O59" s="4">
+      <c r="P59" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P59" s="4">
+      <c r="Q59" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q59" s="4">
+      <c r="R59" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5911,7 +6095,7 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3" t="s">
@@ -5921,40 +6105,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J60" s="2" t="str">
+      <c r="J60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K60" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L60" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D60&amp;" - "&amp;TEXT(F60,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L60" s="4" t="e">
+      <c r="M60" s="4" t="e">
         <f>VLOOKUP(C60,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M60" s="4" t="e">
+      <c r="N60" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N60" s="4">
+      <c r="O60" s="4">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
-      <c r="O60" s="4">
+      <c r="P60" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P60" s="4">
+      <c r="Q60" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q60" s="4">
+      <c r="R60" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5973,7 +6160,7 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3" t="s">
@@ -5983,40 +6170,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J61" s="2" t="str">
+      <c r="J61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K61" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K61" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L61" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D61&amp;" - "&amp;TEXT(F61,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L61" s="4" t="e">
+      <c r="M61" s="4" t="e">
         <f>VLOOKUP(C61,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M61" s="4" t="e">
+      <c r="N61" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N61" s="4">
+      <c r="O61" s="4">
         <f t="shared" si="11"/>
         <v>61</v>
       </c>
-      <c r="O61" s="4">
+      <c r="P61" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P61" s="4">
+      <c r="Q61" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q61" s="4">
+      <c r="R61" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6035,7 +6225,7 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3" t="s">
@@ -6045,40 +6235,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J62" s="2" t="str">
+      <c r="J62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K62" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K62" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L62" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D62&amp;" - "&amp;TEXT(F62,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L62" s="4" t="e">
+      <c r="M62" s="4" t="e">
         <f>VLOOKUP(C62,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M62" s="4" t="e">
+      <c r="N62" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N62" s="4">
+      <c r="O62" s="4">
         <f t="shared" si="11"/>
         <v>62</v>
       </c>
-      <c r="O62" s="4">
+      <c r="P62" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P62" s="4">
+      <c r="Q62" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q62" s="4">
+      <c r="R62" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6097,7 +6290,7 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3" t="s">
@@ -6107,40 +6300,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J63" s="2" t="str">
+      <c r="J63" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K63" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L63" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D63&amp;" - "&amp;TEXT(F63,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L63" s="4" t="e">
+      <c r="M63" s="4" t="e">
         <f>VLOOKUP(C63,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M63" s="4" t="e">
+      <c r="N63" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N63" s="4">
+      <c r="O63" s="4">
         <f t="shared" si="11"/>
         <v>63</v>
       </c>
-      <c r="O63" s="4">
+      <c r="P63" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P63" s="4">
+      <c r="Q63" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q63" s="4">
+      <c r="R63" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6159,7 +6355,7 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3" t="s">
@@ -6169,40 +6365,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J64" s="2" t="str">
+      <c r="J64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K64" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K64" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L64" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D64&amp;" - "&amp;TEXT(F64,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L64" s="4" t="e">
+      <c r="M64" s="4" t="e">
         <f>VLOOKUP(C64,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M64" s="4" t="e">
+      <c r="N64" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N64" s="4">
+      <c r="O64" s="4">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-      <c r="O64" s="4">
+      <c r="P64" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P64" s="4">
+      <c r="Q64" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q64" s="4">
+      <c r="R64" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6221,7 +6420,7 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3" t="s">
@@ -6231,40 +6430,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J65" s="2" t="str">
+      <c r="J65" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K65" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K65" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L65" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D65&amp;" - "&amp;TEXT(F65,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L65" s="4" t="e">
+      <c r="M65" s="4" t="e">
         <f>VLOOKUP(C65,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M65" s="4" t="e">
+      <c r="N65" s="4" t="e">
         <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="N65" s="4">
+      <c r="O65" s="4">
         <f t="shared" si="11"/>
         <v>65</v>
       </c>
-      <c r="O65" s="4">
+      <c r="P65" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P65" s="4">
+      <c r="Q65" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q65" s="4">
+      <c r="R65" s="4">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6283,7 +6485,7 @@
       </c>
       <c r="F66" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3" t="s">
@@ -6293,40 +6495,43 @@
         <f t="shared" si="7"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J66" s="2" t="str">
+      <c r="J66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K66" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L66" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D66&amp;" - "&amp;TEXT(F66,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L66" s="4" t="e">
+      <c r="M66" s="4" t="e">
         <f>VLOOKUP(C66,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M66" s="4" t="e">
-        <f t="shared" ref="M66:M97" si="15">IF(EXACT(L66,E66),"ü","x")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N66" s="4">
+      <c r="N66" s="4" t="e">
+        <f t="shared" ref="N66:N69" si="15">IF(EXACT(M66,E66),"ü","x")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O66" s="4">
         <f t="shared" si="11"/>
         <v>66</v>
       </c>
-      <c r="O66" s="4">
+      <c r="P66" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P66" s="4">
+      <c r="Q66" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q66" s="4">
-        <f t="shared" ref="Q66:Q69" si="16">SUM(O66:P66)</f>
+      <c r="R66" s="4">
+        <f t="shared" ref="R66:R69" si="16">SUM(P66:Q66)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6345,7 +6550,7 @@
       </c>
       <c r="F67" s="3">
         <f t="shared" ref="F67:F69" ca="1" si="17">TODAY()</f>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3" t="s">
@@ -6355,40 +6560,43 @@
         <f t="shared" ref="I67:I69" si="18">H67&amp;B67&amp;"\"</f>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J67" s="2" t="str">
-        <f t="shared" ref="J67:J69" ca="1" si="19">CONCATENATE(TEXT(A67,"0")," - ","CT - ",SUBSTITUTE(D67,"-","")," - ",B67," - ",YEAR(F67)&amp;"-"&amp;TEXT(MONTH(F67),"00")&amp;"-"&amp;TEXT(DAY(F67),"00"),".xlsx")</f>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K67" s="5" t="str">
+      <c r="J67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K67" s="2" t="str">
+        <f t="shared" ref="K67:K69" ca="1" si="19">CONCATENATE(TEXT(A67,"0")," - ","CT - ",SUBSTITUTE(D67,"-","")," - ",B67," - ",YEAR(F67)&amp;"-"&amp;TEXT(MONTH(F67),"00")&amp;"-"&amp;TEXT(DAY(F67),"00"),".xlsx")</f>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L67" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D67&amp;" - "&amp;TEXT(F67,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L67" s="4" t="e">
+      <c r="M67" s="4" t="e">
         <f>VLOOKUP(C67,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M67" s="4" t="e">
+      <c r="N67" s="4" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
-      <c r="N67" s="4">
+      <c r="O67" s="4">
         <f t="shared" si="11"/>
         <v>67</v>
       </c>
-      <c r="O67" s="4">
+      <c r="P67" s="4">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="P67" s="4">
+      <c r="Q67" s="4">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="Q67" s="4">
+      <c r="R67" s="4">
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6407,7 +6615,7 @@
       </c>
       <c r="F68" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3" t="s">
@@ -6417,40 +6625,43 @@
         <f t="shared" si="18"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J68" s="2" t="str">
+      <c r="J68" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" s="2" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K68" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L68" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D68&amp;" - "&amp;TEXT(F68,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L68" s="4" t="e">
+      <c r="M68" s="4" t="e">
         <f>VLOOKUP(C68,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M68" s="4" t="e">
+      <c r="N68" s="4" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
-      <c r="N68" s="4">
+      <c r="O68" s="4">
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
-      <c r="O68" s="4">
-        <f t="shared" ref="O68:O69" si="20">IF(C68=C67,1,0)</f>
-        <v>1</v>
-      </c>
       <c r="P68" s="4">
-        <f t="shared" ref="P68:P69" si="21">IF(C68=C69,1,0)</f>
+        <f t="shared" ref="P68:P69" si="20">IF(C68=C67,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q68" s="4">
+        <f t="shared" ref="Q68:Q69" si="21">IF(C68=C69,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R68" s="4">
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6469,7 +6680,7 @@
       </c>
       <c r="F69" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45109</v>
+        <v>45254</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3" t="s">
@@ -6479,45 +6690,53 @@
         <f t="shared" si="18"/>
         <v>F:\Proyecto Uipath\Descarga-de-Cuentas-Tributarias\Test\Cliente\</v>
       </c>
-      <c r="J69" s="2" t="str">
+      <c r="J69" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" s="2" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-07-02.xlsx</v>
-      </c>
-      <c r="K69" s="5" t="str">
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+      </c>
+      <c r="L69" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D69&amp;" - "&amp;TEXT(F69,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
         <v/>
       </c>
-      <c r="L69" s="4" t="e">
+      <c r="M69" s="4" t="e">
         <f>VLOOKUP(C69,[2]Hoja1!$J:$L,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M69" s="4" t="e">
+      <c r="N69" s="4" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
-      <c r="N69" s="4">
+      <c r="O69" s="4">
         <f t="shared" si="11"/>
         <v>69</v>
       </c>
-      <c r="O69" s="4">
+      <c r="P69" s="4">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="P69" s="4">
+      <c r="Q69" s="4">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Q69" s="4">
+      <c r="R69" s="4">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N69">
+  <autoFilter ref="A1:R69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O69">
     <sortCondition ref="A2:A69"/>
     <sortCondition ref="D2:D69"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J69" xr:uid="{F5AE022F-379C-49A3-9812-603ACB4E2D56}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Change .xlsx for .csv
</commit_message>
<xml_diff>
--- a/Listado CT.xlsx
+++ b/Listado CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Descarga-de-Cuentas-Tributarias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D787A2D-F7AB-47F2-816A-84CB6D093535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2AC83C-47A7-4026-8E9F-878CFE52F30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2333,8 +2333,8 @@
         <v>20</v>
       </c>
       <c r="K2" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CT - ",SUBSTITUTE(D2,"-","")," - ",B2," - ",YEAR(F2)&amp;"-"&amp;TEXT(MONTH(F2),"00")&amp;"-"&amp;TEXT(DAY(F2),"00"),".xlsx")</f>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CT - ",SUBSTITUTE(D2,"-","")," - ",B2," - ",YEAR(F2)&amp;"-"&amp;TEXT(MONTH(F2),"00")&amp;"-"&amp;TEXT(DAY(F2),"00"),".csv")</f>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L2" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D2&amp;" - "&amp;TEXT(F2,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2399,8 +2399,8 @@
         <v>20</v>
       </c>
       <c r="K3" s="2" t="str">
-        <f t="shared" ref="K3:K66" ca="1" si="8">CONCATENATE(TEXT(A3,"0")," - ","CT - ",SUBSTITUTE(D3,"-","")," - ",B3," - ",YEAR(F3)&amp;"-"&amp;TEXT(MONTH(F3),"00")&amp;"-"&amp;TEXT(DAY(F3),"00"),".xlsx")</f>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <f t="shared" ref="K3:K66" ca="1" si="8">CONCATENATE(TEXT(A3,"0")," - ","CT - ",SUBSTITUTE(D3,"-","")," - ",B3," - ",YEAR(F3)&amp;"-"&amp;TEXT(MONTH(F3),"00")&amp;"-"&amp;TEXT(DAY(F3),"00"),".csv")</f>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L3" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D3&amp;" - "&amp;TEXT(F3,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="K4" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L4" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D4&amp;" - "&amp;TEXT(F4,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="K5" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L5" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D5&amp;" - "&amp;TEXT(F5,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L6" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D6&amp;" - "&amp;TEXT(F6,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="K7" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L7" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D7&amp;" - "&amp;TEXT(F7,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="K8" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L8" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D8&amp;" - "&amp;TEXT(F8,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="K9" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 20000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L9" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D9&amp;" - "&amp;TEXT(F9,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="K10" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L10" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D10&amp;" - "&amp;TEXT(F10,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="K11" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L11" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D11&amp;" - "&amp;TEXT(F11,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="K12" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L12" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D12&amp;" - "&amp;TEXT(F12,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L13" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D13&amp;" - "&amp;TEXT(F13,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L14" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D14&amp;" - "&amp;TEXT(F14,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L15" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D15&amp;" - "&amp;TEXT(F15,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L16" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D16&amp;" - "&amp;TEXT(F16,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="K17" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L17" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D17&amp;" - "&amp;TEXT(F17,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="K18" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L18" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D18&amp;" - "&amp;TEXT(F18,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="K19" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L19" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D19&amp;" - "&amp;TEXT(F19,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="K20" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L20" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D20&amp;" - "&amp;TEXT(F20,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="K21" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L21" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D21&amp;" - "&amp;TEXT(F21,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L22" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D22&amp;" - "&amp;TEXT(F22,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="K23" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L23" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D23&amp;" - "&amp;TEXT(F23,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="K24" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L24" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D24&amp;" - "&amp;TEXT(F24,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="K25" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L25" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D25&amp;" - "&amp;TEXT(F25,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L26" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D26&amp;" - "&amp;TEXT(F26,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="K27" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L27" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D27&amp;" - "&amp;TEXT(F27,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="K28" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L28" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D28&amp;" - "&amp;TEXT(F28,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="K29" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L29" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D29&amp;" - "&amp;TEXT(F29,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="K30" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L30" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D30&amp;" - "&amp;TEXT(F30,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="K31" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L31" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D31&amp;" - "&amp;TEXT(F31,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="K32" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L32" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D32&amp;" - "&amp;TEXT(F32,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4355,7 +4355,7 @@
       </c>
       <c r="K33" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L33" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D33&amp;" - "&amp;TEXT(F33,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="K34" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L34" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D34&amp;" - "&amp;TEXT(F34,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4485,7 +4485,7 @@
       </c>
       <c r="K35" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L35" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D35&amp;" - "&amp;TEXT(F35,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="K36" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L36" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D36&amp;" - "&amp;TEXT(F36,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4615,7 +4615,7 @@
       </c>
       <c r="K37" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L37" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D37&amp;" - "&amp;TEXT(F37,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="K38" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L38" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D38&amp;" - "&amp;TEXT(F38,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4745,7 +4745,7 @@
       </c>
       <c r="K39" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L39" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D39&amp;" - "&amp;TEXT(F39,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L40" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D40&amp;" - "&amp;TEXT(F40,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="K41" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L41" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D41&amp;" - "&amp;TEXT(F41,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="K42" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L42" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D42&amp;" - "&amp;TEXT(F42,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="K43" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L43" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D43&amp;" - "&amp;TEXT(F43,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="K44" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L44" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D44&amp;" - "&amp;TEXT(F44,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="K45" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L45" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D45&amp;" - "&amp;TEXT(F45,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="K46" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L46" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D46&amp;" - "&amp;TEXT(F46,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="K47" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L47" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D47&amp;" - "&amp;TEXT(F47,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="K48" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L48" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D48&amp;" - "&amp;TEXT(F48,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5395,7 +5395,7 @@
       </c>
       <c r="K49" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L49" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D49&amp;" - "&amp;TEXT(F49,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="K50" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L50" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D50&amp;" - "&amp;TEXT(F50,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="K51" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L51" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D51&amp;" - "&amp;TEXT(F51,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="K52" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L52" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D52&amp;" - "&amp;TEXT(F52,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="K53" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L53" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D53&amp;" - "&amp;TEXT(F53,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="K54" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L54" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D54&amp;" - "&amp;TEXT(F54,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="K55" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L55" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D55&amp;" - "&amp;TEXT(F55,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5850,7 +5850,7 @@
       </c>
       <c r="K56" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L56" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D56&amp;" - "&amp;TEXT(F56,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="K57" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L57" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D57&amp;" - "&amp;TEXT(F57,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="K58" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L58" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D58&amp;" - "&amp;TEXT(F58,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="K59" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L59" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D59&amp;" - "&amp;TEXT(F59,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="K60" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L60" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D60&amp;" - "&amp;TEXT(F60,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="K61" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L61" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D61&amp;" - "&amp;TEXT(F61,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="K62" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L62" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D62&amp;" - "&amp;TEXT(F62,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="K63" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L63" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D63&amp;" - "&amp;TEXT(F63,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6370,7 +6370,7 @@
       </c>
       <c r="K64" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L64" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D64&amp;" - "&amp;TEXT(F64,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="K65" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L65" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D65&amp;" - "&amp;TEXT(F65,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6500,7 +6500,7 @@
       </c>
       <c r="K66" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L66" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D66&amp;" - "&amp;TEXT(F66,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6564,8 +6564,8 @@
         <v>20</v>
       </c>
       <c r="K67" s="2" t="str">
-        <f t="shared" ref="K67:K69" ca="1" si="19">CONCATENATE(TEXT(A67,"0")," - ","CT - ",SUBSTITUTE(D67,"-","")," - ",B67," - ",YEAR(F67)&amp;"-"&amp;TEXT(MONTH(F67),"00")&amp;"-"&amp;TEXT(DAY(F67),"00"),".xlsx")</f>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <f t="shared" ref="K67:K69" ca="1" si="19">CONCATENATE(TEXT(A67,"0")," - ","CT - ",SUBSTITUTE(D67,"-","")," - ",B67," - ",YEAR(F67)&amp;"-"&amp;TEXT(MONTH(F67),"00")&amp;"-"&amp;TEXT(DAY(F67),"00"),".csv")</f>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L67" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D67&amp;" - "&amp;TEXT(F67,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="K68" s="2" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L68" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D68&amp;" - "&amp;TEXT(F68,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>
@@ -6695,7 +6695,7 @@
       </c>
       <c r="K69" s="2" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.xlsx</v>
+        <v>0 - CT - 30000000000 - Cliente - 2023-11-24.csv</v>
       </c>
       <c r="L69" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D69&amp;" - "&amp;TEXT(F69,"aaaa-mm-dd"),[1]Control!$C:$D,2,0),"")</f>

</xml_diff>